<commit_message>
Excluded protocol.id from mwtab, lots of testing files and example changes.
</commit_message>
<xml_diff>
--- a/examples/Full_mwtab_example/NMR/extract/NMR_colon_measurements.xlsx
+++ b/examples/Full_mwtab_example/NMR/extract/NMR_colon_measurements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sparda\Desktop\Moseley Lab\Code\MESSES\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sparda\Desktop\Moseley Lab\Code\MESSES\examples\Full_mwtab_example\NMR\extract\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD65895B-0A77-4701-9647-0036A98A0F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01C7131-7BFE-462E-A9C9-FA39FEC70328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4710" yWindow="2220" windowWidth="21720" windowHeight="12975" xr2:uid="{432708A5-97B1-49E8-8A1C-5E278420EF0F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{432708A5-97B1-49E8-8A1C-5E278420EF0F}"/>
   </bookViews>
   <sheets>
     <sheet name="#automate" sheetId="3" r:id="rId1"/>
@@ -2305,7 +2305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645C32B4-4612-4621-9B73-94B95602C2C8}">
   <dimension ref="A1:W36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -74050,15 +74050,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6103AD33-330F-4815-96B0-5CF8C0E460E2}">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>123</v>
       </c>
@@ -74078,7 +74078,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>30</v>
       </c>
@@ -74089,7 +74089,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>31</v>
       </c>
@@ -74100,7 +74100,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>19</v>
       </c>
@@ -74111,7 +74111,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>20</v>
       </c>
@@ -74122,7 +74122,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>89</v>
       </c>
@@ -74133,7 +74133,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>597</v>
       </c>
@@ -74144,7 +74144,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>598</v>
       </c>
@@ -74155,7 +74155,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>107</v>
       </c>
@@ -74166,7 +74166,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>123</v>
       </c>
@@ -74186,7 +74186,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>105</v>
       </c>
@@ -74196,8 +74196,12 @@
       <c r="F13" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S13" t="str">
+        <f>_xlfn.CONCAT("r'",B13,"',r'",C13,"'")</f>
+        <v>r'01_A0_13C6-Glc_UKy_GCH_Ms_colon_PRESAT_01',r'01_A0_Colon_naive_0days_170427_UKy_GCH_rep1-polar-NMR_A'</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>108</v>
       </c>
@@ -74207,8 +74211,12 @@
       <c r="F14" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S14" t="str">
+        <f t="shared" ref="S14:S27" si="0">_xlfn.CONCAT("r'",B14,"',r'",C14,"'")</f>
+        <v>r'02_A1_13C6-Glc_UKy_GCH_Ms_colon_PRESAT_01',r'02_A1_Colon_naive_0days_170427_UKy_GCH_rep2-polar-NMR_A'</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>109</v>
       </c>
@@ -74218,8 +74226,12 @@
       <c r="F15" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S15" t="str">
+        <f t="shared" si="0"/>
+        <v>r'03_A2_13C6-Glc_UKy_GCH_Ms_colon_PRESAT_01',r'03_A2_Colon_naive_0days_170427_UKy_GCH_rep3-polar-NMR_A'</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>110</v>
       </c>
@@ -74229,8 +74241,12 @@
       <c r="F16" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="S16" t="str">
+        <f t="shared" si="0"/>
+        <v>r'04_B0_13C6-Glc_UKy_GCH_Ms_colon_PRESAT_01',r'04_B0_Colon_syngenic_42days_170427_UKy_GCH_rep1-polar-NMR_A'</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>111</v>
       </c>
@@ -74240,8 +74256,12 @@
       <c r="F17" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="S17" t="str">
+        <f t="shared" si="0"/>
+        <v>r'05_B1_13C6-Glc_UKy_GCH_Ms_colon_PRESAT_01',r'05_B1_Colon_syngenic_42days_170427_UKy_GCH_rep2-polar-NMR_A'</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>112</v>
       </c>
@@ -74251,8 +74271,12 @@
       <c r="F18" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="S18" t="str">
+        <f t="shared" si="0"/>
+        <v>r'06_B2_13C6-Glc_UKy_GCH_Ms_colon_PRESAT_01',r'06_B2_Colon_syngenic_42days_170427_UKy_GCH_rep3-polar-NMR_A'</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>113</v>
       </c>
@@ -74262,8 +74286,12 @@
       <c r="F19" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="S19" t="str">
+        <f t="shared" si="0"/>
+        <v>r'07_C1-1_13C6-Glc_UKy_GCH_Ms_colon_PRESAT_01',r'07_C1-1_Colon_allogenic_42days_170427_UKy_GCH_rep1-polar-NMR_A'</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>114</v>
       </c>
@@ -74273,8 +74301,12 @@
       <c r="F20" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="S20" t="str">
+        <f t="shared" si="0"/>
+        <v>r'08_C1-2_13C6-Glc_UKy_GCH_Ms_colon_PRESAT_01',r'08_C1-2_Colon_allogenic_42days_170427_UKy_GCH_rep2-polar-NMR_A'</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>115</v>
       </c>
@@ -74284,8 +74316,12 @@
       <c r="F21" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="S21" t="str">
+        <f t="shared" si="0"/>
+        <v>r'09_C2-0_13C6-Glc_UKy_GCH_Ms_colon_PRESAT_01',r'09_C2-0_Colon_allogenic_42days_170427_UKy_GCH_rep1-polar-NMR_A'</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>116</v>
       </c>
@@ -74295,8 +74331,12 @@
       <c r="F22" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="S22" t="str">
+        <f t="shared" si="0"/>
+        <v>r'10_B1-0_13C6-Glc_UKy_GCH_Ms_colon_PRESAT_01',r'10_B1-0_Colon_syngenic_7days_170427_UKy_GCH_rep1-polar-NMR_A'</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>117</v>
       </c>
@@ -74306,8 +74346,12 @@
       <c r="F23" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="S23" t="str">
+        <f t="shared" si="0"/>
+        <v>r'11_B1-1_13C6-Glc_UKy_GCH_Ms_colon_PRESAT_01',r'11_B1-1_Colon_syngenic_7days_170427_UKy_GCH_rep2-polar-NMR_A'</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>118</v>
       </c>
@@ -74317,8 +74361,12 @@
       <c r="F24" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="S24" t="str">
+        <f t="shared" si="0"/>
+        <v>r'12_B1-2_13C6-Glc_UKy_GCH_Ms_colon_PRESAT_01',r'12_B1-2_Colon_syngenic_7days_170427_UKy_GCH_rep3-polar-NMR_A'</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>119</v>
       </c>
@@ -74328,8 +74376,12 @@
       <c r="F25" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="S25" t="str">
+        <f t="shared" si="0"/>
+        <v>r'13_C1-1_13C6-Glc_UKy_GCH_Ms_colon_PRESAT_01',r'13_C1-1_Colon_allogenic_7days_170427_UKy_GCH_rep1-polar-NMR_A'</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>120</v>
       </c>
@@ -74339,8 +74391,12 @@
       <c r="F26" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="S26" t="str">
+        <f t="shared" si="0"/>
+        <v>r'14_C1-2_13C6-Glc_UKy_GCH_Ms_colon_PRESAT_01',r'14_C1-2_Colon_allogenic_7days_170427_UKy_GCH_rep2-polar-NMR_A'</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>121</v>
       </c>
@@ -74349,6 +74405,10 @@
       </c>
       <c r="F27" t="s">
         <v>596</v>
+      </c>
+      <c r="S27" t="str">
+        <f t="shared" si="0"/>
+        <v>r'15_C1-20_13C6-Glc_UKy_GCH_Ms_colon_PRESAT_01',r'15_C1-20_Colon_allogenic_7days_170427_UKy_GCH_rep3-polar-NMR_A'</v>
       </c>
     </row>
   </sheetData>

</xml_diff>